<commit_message>
Update options in menu, implement previous labels
</commit_message>
<xml_diff>
--- a/visualizer/visualizerLabels.xlsx
+++ b/visualizer/visualizerLabels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\okrahR\msm-visualizer\visualizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\OneDrive\11_Nuevos_proyectos\MSM\msmvisualizer\visualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89F4494-AD56-4BBE-8404-DD845B045447}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C89F4494-AD56-4BBE-8404-DD845B045447}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A593C055-351C-44E1-9013-477428A9067F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{247ECA27-6467-44D0-B0C0-41F1584AA2D9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{247ECA27-6467-44D0-B0C0-41F1584AA2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -840,22 +840,24 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="33.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="9" max="12" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -893,7 +895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -925,7 +927,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -963,7 +965,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1001,7 +1003,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1126,7 +1128,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1158,7 +1160,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1196,7 +1198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1342,7 +1344,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1441,7 +1443,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1505,7 +1507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1537,7 +1539,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1569,7 +1571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1601,7 +1603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1633,7 +1635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1805,7 +1807,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -1854,7 +1856,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1871,7 +1873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1888,7 +1890,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -1905,7 +1907,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -1922,7 +1924,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -1939,7 +1941,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1956,7 +1958,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1990,7 +1992,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2007,7 +2009,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2024,7 +2026,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -2041,7 +2043,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -2092,7 +2094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>118</v>
       </c>
@@ -2138,7 +2140,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -2167,7 +2169,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -2225,7 +2227,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>118</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>123</v>
       </c>
@@ -2288,7 +2290,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>123</v>
       </c>
@@ -2305,7 +2307,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>123</v>
       </c>

</xml_diff>